<commit_message>
Se realizan ajustes a los casos de usos
</commit_message>
<xml_diff>
--- a/Propuesta/CasosUsos/Caso de Uso 1 Login.xlsx
+++ b/Propuesta/CasosUsos/Caso de Uso 1 Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imroo\Desktop\SIS\CompuMovil\Proyecto\computacion_movil\Propuesta\CasosUsos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Javeriana\Semestre 1\ComputacionMovil\Proyecto\computacion_movil\Propuesta\CasosUsos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2106B28A-AB66-43D6-B791-C1B2B7AAAC86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C680AA-9D39-43FA-8A46-F6C14652F3A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="450" windowWidth="28620" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$F$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$F$65</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Hoja1!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
-  <si>
-    <t>Módulo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Datos de Entrada</t>
   </si>
@@ -209,7 +206,31 @@
     <t>Iniciar sesion.</t>
   </si>
   <si>
-    <t>El usuario ingresa sus credenciales en la pantalla para iniciar sesión y utilizas la aplicación.</t>
+    <t>Proyecto</t>
+  </si>
+  <si>
+    <t>Plus E</t>
+  </si>
+  <si>
+    <t>Los que sobran</t>
+  </si>
+  <si>
+    <t>Autenticación de la plataforma</t>
+  </si>
+  <si>
+    <t>Event Plus</t>
+  </si>
+  <si>
+    <t>Icono</t>
+  </si>
+  <si>
+    <t>Nombre Equipo</t>
+  </si>
+  <si>
+    <t>Nombre Materia</t>
+  </si>
+  <si>
+    <t>Carlos Parra</t>
   </si>
 </sst>
 </file>
@@ -234,10 +255,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -588,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -599,12 +622,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -704,17 +721,122 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -724,102 +846,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,23 +868,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>548610</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>230904</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1106130</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>163871</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>63114</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>1754454</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>594033</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1701326</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A11A76D6-C27F-4882-90B4-EA90F5D9F7AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B95DA9A-3203-4699-B96B-D4CA42D41FFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -874,8 +900,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1931271" y="5423565"/>
-          <a:ext cx="2279827" cy="3602663"/>
+          <a:off x="5254114" y="6134919"/>
+          <a:ext cx="2253225" cy="3616568"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -886,23 +912,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1101674</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>241145</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1218792</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>245807</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>648399</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>1764695</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>335287</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1679678</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FD0904F-6A8C-4933-B4E8-3896E7380F1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5305189E-E4DD-4EB8-82C3-5A2C28338EC7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -918,12 +944,19 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5249658" y="5433806"/>
-          <a:ext cx="2312047" cy="3602663"/>
+          <a:off x="2601453" y="6216855"/>
+          <a:ext cx="1881818" cy="3512984"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1252,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:H61"/>
+  <dimension ref="A4:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="93" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:F10"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="93" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1266,295 +1299,303 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
+      <c r="A4" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="63"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="63"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63"/>
+    </row>
+    <row r="12" spans="1:6" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="63"/>
+    </row>
+    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="63"/>
+    </row>
+    <row r="14" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="53"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="66"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="50"/>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="77"/>
+      <c r="B17" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="63"/>
+    </row>
+    <row r="18" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="78"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="66"/>
+    </row>
+    <row r="19" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
+    </row>
+    <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="77"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="63"/>
+    </row>
+    <row r="21" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="78"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="66"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="60"/>
+    </row>
+    <row r="23" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="52"/>
+      <c r="B23" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="52"/>
+      <c r="B24" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
-    </row>
-    <row r="8" spans="1:6" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
-    </row>
-    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="47"/>
-    </row>
-    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="49"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-    </row>
-    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="C24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="6">
+        <v>20</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="52"/>
+      <c r="B25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="6">
         <v>8</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
-    </row>
-    <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
-      <c r="B13" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="47"/>
-    </row>
-    <row r="14" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-    </row>
-    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
-    </row>
-    <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
-    </row>
-    <row r="17" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="56" t="s">
+      <c r="E25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="52"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="52"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="52"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="52"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:8" ht="163.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="52"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="71"/>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="52"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="74"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="52"/>
+      <c r="B32" s="58" t="s">
         <v>9</v>
-      </c>
-      <c r="B18" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="60"/>
-    </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="49"/>
-      <c r="B19" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
-      <c r="B20" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="8">
-        <v>20</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="8">
-        <v>8</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="49"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:8" ht="163.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
-      <c r="B26" s="68"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="70"/>
-      <c r="H26"/>
-    </row>
-    <row r="27" spans="1:8" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="73"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
-      <c r="B28" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="60"/>
-    </row>
-    <row r="29" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="47"/>
-    </row>
-    <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="49"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="47"/>
-    </row>
-    <row r="31" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="49"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="40"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="49"/>
-      <c r="B32" s="58" t="s">
-        <v>11</v>
       </c>
       <c r="C32" s="59"/>
       <c r="D32" s="59"/>
@@ -1562,362 +1603,403 @@
       <c r="F32" s="60"/>
     </row>
     <row r="33" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="49"/>
-      <c r="B33" s="17" t="s">
+      <c r="A33" s="52"/>
+      <c r="B33" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="63"/>
+    </row>
+    <row r="34" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="52"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="63"/>
+    </row>
+    <row r="35" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="52"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="66"/>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="52"/>
+      <c r="B36" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="60"/>
+    </row>
+    <row r="37" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="52"/>
+      <c r="B37" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="D37" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="67"/>
+      <c r="F37" s="68"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="52"/>
+      <c r="B38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="40"/>
+      <c r="F38" s="41"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="52"/>
+      <c r="B39" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="40"/>
+      <c r="F39" s="41"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="52"/>
+      <c r="B40" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="40"/>
+      <c r="F40" s="41"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="52"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="41"/>
+    </row>
+    <row r="42" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="52"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="41"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="53"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="43"/>
+    </row>
+    <row r="44" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="63" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="64"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="49"/>
-      <c r="B34" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="65" t="s">
+      <c r="C44" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="45"/>
+      <c r="F44" s="46"/>
+    </row>
+    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="52"/>
+      <c r="B45" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="40"/>
+      <c r="F45" s="41"/>
+    </row>
+    <row r="46" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="52"/>
+      <c r="B46" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="51"/>
-      <c r="F34" s="52"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="49"/>
-      <c r="B35" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="51"/>
-      <c r="F35" s="52"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="49"/>
-      <c r="B36" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" s="51"/>
-      <c r="F36" s="52"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="49"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="52"/>
-    </row>
-    <row r="38" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="49"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="52"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="57"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="55"/>
-    </row>
-    <row r="40" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="56" t="s">
+      <c r="C46" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="40"/>
+      <c r="F46" s="41"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="52"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="41"/>
+    </row>
+    <row r="48" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="53"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="43"/>
+    </row>
+    <row r="49" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="48"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="50"/>
+    </row>
+    <row r="50" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="52"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="63"/>
+    </row>
+    <row r="51" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="53"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="65"/>
+      <c r="D51" s="65"/>
+      <c r="E51" s="65"/>
+      <c r="F51" s="66"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="47"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+    </row>
+    <row r="53" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" s="66"/>
-      <c r="F40" s="67"/>
-    </row>
-    <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="49"/>
-      <c r="B41" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" s="65" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="51"/>
-      <c r="F41" s="52"/>
-    </row>
-    <row r="42" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="49"/>
-      <c r="B42" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" s="51"/>
-      <c r="F42" s="52"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="49"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="52"/>
-    </row>
-    <row r="44" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="57"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="55"/>
-    </row>
-    <row r="45" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="B45" s="53"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="42"/>
-    </row>
-    <row r="46" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="49"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="47"/>
-    </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="57"/>
-      <c r="B47" s="62"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="40"/>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-    </row>
-    <row r="49" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="56" t="s">
+      <c r="C53" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="52"/>
+      <c r="B54" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" s="26"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="52"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="52"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="52"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="52"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="53"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="11"/>
+    </row>
+    <row r="60" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="F49" s="30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="49"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="E50" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="F50" s="28"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="49"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="11"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="49"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="11"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="49"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="11"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="49"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="11"/>
-    </row>
-    <row r="55" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="57"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="13"/>
-    </row>
-    <row r="56" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="B56" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="29" t="s">
+      <c r="E60" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="D56" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="74" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" s="75"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="49"/>
-      <c r="B57" s="32"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="76"/>
-      <c r="F57" s="77"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="49"/>
-      <c r="B58" s="33"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="51"/>
-      <c r="F58" s="52"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="49"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="51"/>
-      <c r="F59" s="52"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="49"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="51"/>
-      <c r="F60" s="52"/>
-    </row>
-    <row r="61" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="57"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="54"/>
-      <c r="F61" s="55"/>
+      <c r="F60" s="55"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="52"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="56"/>
+      <c r="F61" s="57"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="52"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="41"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="52"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="41"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="52"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="41"/>
+    </row>
+    <row r="65" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="53"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="A56:A61"/>
-    <mergeCell ref="A49:A55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
+  <mergeCells count="50">
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B13:F14"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
     <mergeCell ref="E60:F60"/>
-    <mergeCell ref="B26:F27"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A22:A43"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F35"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="B30:F31"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
     <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="B49:F49"/>
     <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="A48:F48"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A18:A39"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F31"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="A60:A65"/>
+    <mergeCell ref="A53:A59"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>